<commit_message>
add one more example
</commit_message>
<xml_diff>
--- a/CodeKata-core/src/test/java/kata/excel/ExcelBDD.xlsx
+++ b/CodeKata-core/src/test/java/kata/excel/ExcelBDD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VSCode\SimpleOpen\ScrumBan\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\git\CodeKata\CodeKata-core\src\test\java\kata\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36CB77B-3382-4F27-BD9B-C1846495C895}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A430A62-E059-4E93-9246-F6CA9FBCEE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleOpenBDD" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="7" r:id="rId6"/>
+    <sheet name="StoryExample1" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="141">
   <si>
     <t>Role</t>
   </si>
@@ -343,13 +344,133 @@
   </si>
   <si>
     <t>2021/4/30</t>
+  </si>
+  <si>
+    <t>filter the dashboard by department</t>
+  </si>
+  <si>
+    <t>As an executive, I want to be able to filter the dashboard by department so that I can isolate data by a specific department.</t>
+  </si>
+  <si>
+    <t>SelectedView</t>
+  </si>
+  <si>
+    <t>Given： go to Executive Dashboard [SelectedView]</t>
+  </si>
+  <si>
+    <t>default view</t>
+  </si>
+  <si>
+    <t>DeptA</t>
+  </si>
+  <si>
+    <t>When: select the department drop-down</t>
+  </si>
+  <si>
+    <t>DepartmentCount</t>
+  </si>
+  <si>
+    <t>SelectedDepartment</t>
+  </si>
+  <si>
+    <t>Then:only that data throughout the dashboard.the entire dashboard filters to display only that department data</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>When: select one depart [SelectedDepartment]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A department list appears with [DepartmentCount] departments</t>
+  </si>
+  <si>
+    <t>Show full Name of Department</t>
+  </si>
+  <si>
+    <t>FullDepartmentName</t>
+  </si>
+  <si>
+    <t>Axx&amp;Bxx Dept</t>
+  </si>
+  <si>
+    <t>DepartmentLocation</t>
+  </si>
+  <si>
+    <t>DepartmentCurrentMonthKPI1</t>
+  </si>
+  <si>
+    <t>DepartmentCurrentMonthKPI2</t>
+  </si>
+  <si>
+    <t>Show location</t>
+  </si>
+  <si>
+    <t>Show Current Month KPI1</t>
+  </si>
+  <si>
+    <t>Show Current Month KPI2</t>
+  </si>
+  <si>
+    <t>12%</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>DeptB</t>
+  </si>
+  <si>
+    <t>DeptC</t>
+  </si>
+  <si>
+    <t>CCC Dept</t>
+  </si>
+  <si>
+    <t>BBBB Dept</t>
+  </si>
+  <si>
+    <t>ShengZhen</t>
+  </si>
+  <si>
+    <t>HongKong</t>
+  </si>
+  <si>
+    <t>Scenario5</t>
+  </si>
+  <si>
+    <t>Scenario6</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>ViewA</t>
+  </si>
+  <si>
+    <t>ViewB</t>
+  </si>
+  <si>
+    <t>DeptD</t>
+  </si>
+  <si>
+    <t>DDDept</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>HangZhou</t>
+  </si>
+  <si>
+    <t>NanJing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +506,30 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
@@ -434,7 +579,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -558,13 +703,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -602,75 +791,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -685,18 +805,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -705,6 +813,159 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1122,7 +1383,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1132,12 +1393,12 @@
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="45">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1164,13 +1425,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30">
-      <c r="A2" s="46">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -1190,13 +1451,13 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="46">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1216,13 +1477,13 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
-      <c r="A4" s="46">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -1242,13 +1503,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
-      <c r="A5" s="46">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -1268,13 +1529,13 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="46">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1294,13 +1555,13 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="46">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1320,13 +1581,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="46">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1346,13 +1607,13 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="46">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1372,13 +1633,13 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="46">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1390,13 +1651,13 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" ht="30">
-      <c r="A11" s="46">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1408,75 +1669,75 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="45">
-      <c r="A12" s="50">
+      <c r="A12" s="40">
         <v>11</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="37">
         <v>3</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="37">
         <v>3</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="37">
         <v>3</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="37">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="51"/>
-      <c r="B13" s="44" t="s">
+      <c r="A13" s="41"/>
+      <c r="B13" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="51"/>
-      <c r="B14" s="44" t="s">
+      <c r="A14" s="41"/>
+      <c r="B14" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="52"/>
-      <c r="B15" s="45" t="s">
+      <c r="A15" s="42"/>
+      <c r="B15" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" ht="30">
-      <c r="A16" s="53">
+      <c r="A16" s="26">
         <v>12</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="16" t="s">
@@ -1496,13 +1757,13 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="30">
-      <c r="A17" s="53">
+      <c r="A17" s="26">
         <v>13</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1540,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5657C2-106C-47C7-BF16-329C2F267F09}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1649,7 +1910,7 @@
       <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="47" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1662,7 +1923,7 @@
       <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="28"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -1673,19 +1934,19 @@
       <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="49" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="30" t="s">
         <v>100</v>
       </c>
       <c r="D9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="E9" s="56" t="b">
+      <c r="E9" s="29" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="7">
@@ -1696,7 +1957,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="30"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -1903,7 +2164,7 @@
       <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="30" t="s">
         <v>100</v>
       </c>
       <c r="E9" s="8" t="b">
@@ -1912,7 +2173,7 @@
       <c r="F9" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="56" t="b">
+      <c r="G9" s="29" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="7">
@@ -1920,7 +2181,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="28" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1968,15 +2229,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -2012,7 +2273,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="52" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2038,7 +2299,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -2062,7 +2323,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2082,13 +2343,13 @@
       <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="30" t="s">
         <v>100</v>
       </c>
       <c r="F6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="56" t="b">
+      <c r="G6" s="29" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="7">
@@ -2140,42 +2401,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="51"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="43"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -2207,16 +2468,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="58" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="52" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2236,12 +2497,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="39"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="33"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2259,12 +2520,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="39"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="34"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="54"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -2274,7 +2535,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="40"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
@@ -2287,13 +2548,13 @@
       <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="30" t="s">
         <v>100</v>
       </c>
       <c r="G7" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="56" t="b">
+      <c r="H7" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I7" s="7">
@@ -2347,4 +2608,313 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25">
+      <c r="A1" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+    </row>
+    <row r="2" spans="1:11" ht="38.25" customHeight="1">
+      <c r="A2" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="81"/>
+      <c r="C2" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="79"/>
+      <c r="D3" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1">
+      <c r="A4" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="51.75" customHeight="1">
+      <c r="A5" s="59"/>
+      <c r="B5" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="80"/>
+      <c r="D5" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="32">
+        <v>22</v>
+      </c>
+      <c r="G5" s="32">
+        <v>22</v>
+      </c>
+      <c r="H5" s="32">
+        <v>22</v>
+      </c>
+      <c r="I5" s="32">
+        <v>22</v>
+      </c>
+      <c r="J5" s="32">
+        <v>13</v>
+      </c>
+      <c r="K5" s="32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="33.75" customHeight="1">
+      <c r="A6" s="59"/>
+      <c r="B6" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="31.5">
+      <c r="A7" s="59"/>
+      <c r="B7" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="65"/>
+      <c r="D7" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30">
+      <c r="A8" s="59"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="31.5">
+      <c r="A9" s="59"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="32">
+        <v>345</v>
+      </c>
+      <c r="G9" s="32">
+        <v>567</v>
+      </c>
+      <c r="H9" s="32">
+        <v>2100</v>
+      </c>
+      <c r="I9" s="32">
+        <v>452</v>
+      </c>
+      <c r="J9" s="32">
+        <v>643</v>
+      </c>
+      <c r="K9" s="32">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="31.5">
+      <c r="A10" s="60"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="34">
+        <v>0.45</v>
+      </c>
+      <c r="H10" s="34">
+        <v>0.65</v>
+      </c>
+      <c r="I10" s="34">
+        <v>0.67</v>
+      </c>
+      <c r="J10" s="34">
+        <v>0.45</v>
+      </c>
+      <c r="K10" s="34">
+        <v>0.34</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B7:C10"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel bdd is updated
</commit_message>
<xml_diff>
--- a/CodeKata-core/src/test/java/kata/excel/ExcelBDD.xlsx
+++ b/CodeKata-core/src/test/java/kata/excel/ExcelBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\git\CodeKata\CodeKata-core\src\test\java\kata\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A430A62-E059-4E93-9246-F6CA9FBCEE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C0F204-5FEF-46E3-93EC-A0B3C693076F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
@@ -18,10 +18,11 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="7" r:id="rId6"/>
-    <sheet name="StoryExample1" sheetId="8" r:id="rId7"/>
+    <sheet name="StoryExample1" sheetId="8" r:id="rId6"/>
+    <sheet name="SBT" sheetId="9" r:id="rId7"/>
+    <sheet name="SBTSheet1" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="163">
   <si>
     <t>Role</t>
   </si>
@@ -464,6 +465,72 @@
   </si>
   <si>
     <t>NanJing</t>
+  </si>
+  <si>
+    <t>SBTSheet1</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Test Result</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Header</t>
+  </si>
+  <si>
+    <t>Sub-Step</t>
+  </si>
+  <si>
+    <t>ExcelFileName</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>select file</t>
+  </si>
+  <si>
+    <t>select sheet</t>
+  </si>
+  <si>
+    <t>Get data from Excel</t>
+  </si>
+  <si>
+    <t>Get first Input</t>
+  </si>
+  <si>
+    <t>Get first Expected</t>
+  </si>
+  <si>
+    <t>Get first test result</t>
+  </si>
+  <si>
+    <t>check error</t>
+  </si>
+  <si>
+    <t>FirstInput</t>
+  </si>
+  <si>
+    <t>FirstExpected</t>
+  </si>
+  <si>
+    <t>FirstTestResult</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>FailedWord</t>
+  </si>
+  <si>
+    <t>StepID</t>
   </si>
 </sst>
 </file>
@@ -536,7 +603,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,6 +642,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,7 +832,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -965,6 +1044,35 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1383,7 +1491,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection sqref="A1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1802,7 +1910,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B29" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2599,22 +2707,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2917,4 +3013,506 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
+  <dimension ref="A4:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:6">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="23">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="91"/>
+      <c r="B6" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="23">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="91"/>
+      <c r="B7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="23">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="91"/>
+      <c r="B8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="23">
+        <v>4</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="92" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="23">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="92"/>
+      <c r="B10" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="23">
+        <v>6</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="92"/>
+      <c r="B11" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="23">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="92"/>
+      <c r="B12" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="23">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="92"/>
+      <c r="B13" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="23">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="B1" s="83" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="85"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="85"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="85"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="82" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="82" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="82" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="82" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="82" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="82" t="s">
+        <v>144</v>
+      </c>
+      <c r="L2" s="82" t="s">
+        <v>142</v>
+      </c>
+      <c r="M2" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" s="82" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>C3</f>
+        <v>V1.1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="str">
+        <f>F3</f>
+        <v>V1.2</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="8" t="str">
+        <f>I3</f>
+        <v>V1.3</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="8" t="str">
+        <f>L3</f>
+        <v>V1.4</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f t="shared" ref="D4:D6" si="0">C4</f>
+        <v>V2.1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="str">
+        <f t="shared" ref="G4:G6" si="1">F4</f>
+        <v>V2.2</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="8" t="str">
+        <f t="shared" ref="J4:J6" si="2">I4</f>
+        <v>V2.3</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="8" t="str">
+        <f t="shared" ref="M4:M6" si="3">L4</f>
+        <v>V2.4</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="90" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2021/4/30</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M6" s="8">
+        <f t="shared" si="3"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>